<commit_message>
Fixed the systematic review stats
</commit_message>
<xml_diff>
--- a/2 - Static and dynamic warning colours/Systematic Review - Aposematism AND Warning Colouration.xlsx
+++ b/2 - Static and dynamic warning colours/Systematic Review - Aposematism AND Warning Colouration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mqoutlook-my.sharepoint.com/personal/christopher_irving_mq_edu_au/Documents/Documents/MultiComponentSignals/2 - Static and dynamic warning colours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{60F66345-1BD8-426E-849B-34D1BA0B6DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2E3767E-48CC-4CDB-A50F-D44CB2470E33}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{60F66345-1BD8-426E-849B-34D1BA0B6DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72B8EFF6-9614-488D-AF3C-9DCAEBB713C1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -2680,8 +2680,8 @@
   </sheetPr>
   <dimension ref="A1:L314"/>
   <sheetViews>
-    <sheetView topLeftCell="A258" zoomScale="96" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:S2"/>
+    <sheetView topLeftCell="G1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9013,7 +9013,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9054,21 +9054,21 @@
         <v>193</v>
       </c>
       <c r="C2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E2">
         <v>11</v>
       </c>
       <c r="F2">
         <f>(C2/B2)*100</f>
-        <v>17.098445595854923</v>
+        <v>16.580310880829018</v>
       </c>
       <c r="G2">
         <f>(D2/B2)*100</f>
-        <v>78.238341968911911</v>
+        <v>77.720207253886002</v>
       </c>
       <c r="H2">
         <f>(E2/B2)*100</f>

</xml_diff>

<commit_message>
Figure 6 Legends fix
Moved the internal titles of figure 6 upwards
</commit_message>
<xml_diff>
--- a/2 - Static and dynamic warning colours/Systematic Review - Aposematism AND Warning Colouration.xlsx
+++ b/2 - Static and dynamic warning colours/Systematic Review - Aposematism AND Warning Colouration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mqoutlook-my.sharepoint.com/personal/christopher_irving_mq_edu_au/Documents/Documents/MultiComponentSignals/2 - Static and dynamic warning colours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{60F66345-1BD8-426E-849B-34D1BA0B6DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72B8EFF6-9614-488D-AF3C-9DCAEBB713C1}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{60F66345-1BD8-426E-849B-34D1BA0B6DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AA9B6EC-DCA2-47A5-90C8-A8EEE6ACF4CD}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1060" yWindow="1060" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -2471,6 +2471,865 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Analysis!$C$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Dynamic</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Static</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unsure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Analysis!$C$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-40A0-469F-8B15-ECDC6DC41330}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>377826</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>84483</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>73026</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>128933</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24B52E8A-AC8F-41C6-2BE7-CC794732B80E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2680,8 +3539,8 @@
   </sheetPr>
   <dimension ref="A1:L314"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView zoomScale="96" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9012,8 +9871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6CB0CA-E9A2-4572-8A5B-ADCA4D9803AF}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9077,6 +9936,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>